<commit_message>
frame work for commit
</commit_message>
<xml_diff>
--- a/src/main/resources/project selenium.xlsx
+++ b/src/main/resources/project selenium.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="15300" windowHeight="5385" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="15300" windowHeight="5385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="organization" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Leads" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E16"/>
+  <oleSize ref="A1:H16"/>
 </workbook>
 </file>
 
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>